<commit_message>
Limpieza de repo, se crea analisis
</commit_message>
<xml_diff>
--- a/Modelos.xlsx
+++ b/Modelos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wuser\Documents\UVG\4to Año\Primer Semestre\Inteligencia Artificial\Labs\Lab2\Lab2-RedesNeuronales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E4F059-CDCD-4510-8176-6291E980E382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B528DEB9-AB6D-419F-9BC3-37F34AC482D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,18 +26,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Neuronas ocultas</t>
   </si>
   <si>
-    <t xml:space="preserve">Vueltas </t>
-  </si>
-  <si>
     <t>Efectividad</t>
   </si>
   <si>
     <t>Normalizacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxiter </t>
+  </si>
+  <si>
+    <t>Capas Ocultas</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>T-shirt/top</t>
+  </si>
+  <si>
+    <t>Trouser</t>
+  </si>
+  <si>
+    <t>Pullover</t>
+  </si>
+  <si>
+    <t>Dress</t>
+  </si>
+  <si>
+    <t>Coat</t>
+  </si>
+  <si>
+    <t>Sandal</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Sneaker</t>
+  </si>
+  <si>
+    <t>Bag</t>
+  </si>
+  <si>
+    <t>Ankle boot</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Significado</t>
   </si>
 </sst>
 </file>
@@ -52,15 +95,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,12 +117,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,59 +427,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:F4"/>
+  <dimension ref="B2:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>87.87</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>533</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>88.53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90101929-64E8-4132-8636-CC3632ABB4BD}">
+  <dimension ref="B2:C12"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>130</v>
-      </c>
-      <c r="D3">
-        <v>3000</v>
-      </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-      <c r="F3">
-        <v>87.87</v>
-      </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>533</v>
-      </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4">
-        <v>1000</v>
-      </c>
-      <c r="F4">
-        <v>88.53</v>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>